<commit_message>
changd BP53I to BP531
</commit_message>
<xml_diff>
--- a/info/RtO_proportion_stained_bins.xlsx
+++ b/info/RtO_proportion_stained_bins.xlsx
@@ -122,9 +122,6 @@
     <t>rad50</t>
   </si>
   <si>
-    <t>53bp1</t>
-  </si>
-  <si>
     <t>ctip</t>
   </si>
   <si>
@@ -156,6 +153,9 @@
   </si>
   <si>
     <t>mre11n</t>
+  </si>
+  <si>
+    <t>53bpi</t>
   </si>
 </sst>
 </file>
@@ -840,7 +840,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -913,7 +913,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
@@ -1065,7 +1065,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>17</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>17</v>
@@ -1125,7 +1125,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
@@ -1145,7 +1145,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>17</v>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>17</v>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>17</v>
@@ -1235,7 +1235,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>19</v>
@@ -1257,7 +1257,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>20</v>
@@ -1287,7 +1287,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>17</v>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
@@ -1377,7 +1377,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>19</v>
@@ -1399,7 +1399,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>17</v>
@@ -1429,7 +1429,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>20</v>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>20</v>

</xml_diff>